<commit_message>
add the python script to collect useful information and generate csv
</commit_message>
<xml_diff>
--- a/comparison/comparison.xlsx
+++ b/comparison/comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuliangyong\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\EPFL\course\gsoc\scala-native-autotest\comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C308D21-E41E-4371-8BDC-FF86C1AF29E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89B8436-9DA7-480E-BE6D-7CE59170E944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0F7EB116-8E3E-4DAC-9B80-7CB50F2397D6}"/>
+    <workbookView xWindow="2988" yWindow="1488" windowWidth="17280" windowHeight="9420" xr2:uid="{0F7EB116-8E3E-4DAC-9B80-7CB50F2397D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>bounce.BounceBenchmark</t>
   </si>
@@ -94,6 +94,10 @@
   </si>
   <si>
     <t>inc comp(ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inc comp v2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -545,6 +549,161 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F2B3-4A6C-90B5-E9AAF7EB7738}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>inc comp v2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>bounce.BounceBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brainfuck.BrainfuckBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>cd.CDBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>deltablue.DeltaBlueBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gcbench.GCBenchBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>histogram.Histogram</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>json.JsonBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>kmeans.KmeansBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>list.ListBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mandelbrot.MandelbrotBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>nbody.NbodyBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>permute.PermuteBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>queens.QueensBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>richards.RichardsBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>rsc.RscBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>rsc.cli.Main</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>sudoku.SudokuBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>tracer.TracerBenchmark</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>6542</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6061</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6179</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5851</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5813</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6409</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5897</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5944</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5901</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5931</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5847</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5824</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8221</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7756</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6061</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5473</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B3C1-4F88-A495-3DDEEB1AC4A4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1134,6 +1293,161 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FD64-4516-8707-1A2851169988}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>inc comp v2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$2:$E$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>bounce.BounceBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brainfuck.BrainfuckBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>cd.CDBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>deltablue.DeltaBlueBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gcbench.GCBenchBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>histogram.Histogram</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>json.JsonBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>kmeans.KmeansBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>list.ListBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>mandelbrot.MandelbrotBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>nbody.NbodyBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>permute.PermuteBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>queens.QueensBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>richards.RichardsBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>rsc.RscBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>rsc.cli.Main</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>sudoku.SudokuBenchmark</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>tracer.TracerBenchmark</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1757</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1636</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1626</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1521</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1909</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1610</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1523</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1587</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1527</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1482</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1575</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2990</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1698</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1516</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E3B0-4306-BDE1-2532922F712B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2803,10 +3117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F046F08D-F85D-44BC-BED6-982A55F38414}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2818,23 +3132,30 @@
     <col min="5" max="5" width="27.33203125" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" customWidth="1"/>
     <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
       </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
       <c r="F1" t="s">
         <v>18</v>
       </c>
       <c r="G1" t="s">
         <v>19</v>
       </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2844,6 +3165,9 @@
       <c r="C2">
         <v>7603</v>
       </c>
+      <c r="D2">
+        <v>6542</v>
+      </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
@@ -2853,8 +3177,11 @@
       <c r="G2">
         <v>1940</v>
       </c>
+      <c r="H2">
+        <v>1952</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2864,6 +3191,9 @@
       <c r="C3">
         <v>7079</v>
       </c>
+      <c r="D3">
+        <v>6061</v>
+      </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
@@ -2873,8 +3203,11 @@
       <c r="G3">
         <v>1841</v>
       </c>
+      <c r="H3">
+        <v>1757</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2884,6 +3217,9 @@
       <c r="C4">
         <v>7007</v>
       </c>
+      <c r="D4">
+        <v>6179</v>
+      </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
@@ -2893,8 +3229,11 @@
       <c r="G4">
         <v>1686</v>
       </c>
+      <c r="H4">
+        <v>1636</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2904,6 +3243,9 @@
       <c r="C5">
         <v>6444</v>
       </c>
+      <c r="D5">
+        <v>5851</v>
+      </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -2913,8 +3255,11 @@
       <c r="G5">
         <v>1673</v>
       </c>
+      <c r="H5">
+        <v>1626</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2924,6 +3269,9 @@
       <c r="C6">
         <v>6654</v>
       </c>
+      <c r="D6">
+        <v>5813</v>
+      </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
@@ -2933,8 +3281,11 @@
       <c r="G6">
         <v>1637</v>
       </c>
+      <c r="H6">
+        <v>1521</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2944,6 +3295,9 @@
       <c r="C7">
         <v>7936</v>
       </c>
+      <c r="D7">
+        <v>6409</v>
+      </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
@@ -2953,8 +3307,11 @@
       <c r="G7">
         <v>2144</v>
       </c>
+      <c r="H7">
+        <v>1909</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2964,6 +3321,9 @@
       <c r="C8">
         <v>6800</v>
       </c>
+      <c r="D8">
+        <v>5897</v>
+      </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
@@ -2973,8 +3333,11 @@
       <c r="G8">
         <v>1627</v>
       </c>
+      <c r="H8">
+        <v>1610</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2984,6 +3347,9 @@
       <c r="C9">
         <v>6554</v>
       </c>
+      <c r="D9">
+        <v>5944</v>
+      </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
@@ -2993,8 +3359,11 @@
       <c r="G9">
         <v>1631</v>
       </c>
+      <c r="H9">
+        <v>1512</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3004,6 +3373,9 @@
       <c r="C10">
         <v>6395</v>
       </c>
+      <c r="D10">
+        <v>5901</v>
+      </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
@@ -3013,8 +3385,11 @@
       <c r="G10">
         <v>1598</v>
       </c>
+      <c r="H10">
+        <v>1636</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3024,6 +3399,9 @@
       <c r="C11">
         <v>6334</v>
       </c>
+      <c r="D11">
+        <v>5931</v>
+      </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
@@ -3033,8 +3411,11 @@
       <c r="G11">
         <v>1626</v>
       </c>
+      <c r="H11">
+        <v>1523</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3044,6 +3425,9 @@
       <c r="C12">
         <v>6629</v>
       </c>
+      <c r="D12">
+        <v>5847</v>
+      </c>
       <c r="E12" t="s">
         <v>10</v>
       </c>
@@ -3053,8 +3437,11 @@
       <c r="G12">
         <v>1735</v>
       </c>
+      <c r="H12">
+        <v>1587</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3064,6 +3451,9 @@
       <c r="C13">
         <v>6768</v>
       </c>
+      <c r="D13">
+        <v>5824</v>
+      </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
@@ -3073,8 +3463,11 @@
       <c r="G13">
         <v>1619</v>
       </c>
+      <c r="H13">
+        <v>1527</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3084,6 +3477,9 @@
       <c r="C14">
         <v>6394</v>
       </c>
+      <c r="D14">
+        <v>6007</v>
+      </c>
       <c r="E14" t="s">
         <v>12</v>
       </c>
@@ -3093,8 +3489,11 @@
       <c r="G14">
         <v>1623</v>
       </c>
+      <c r="H14">
+        <v>1482</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3104,6 +3503,9 @@
       <c r="C15">
         <v>6610</v>
       </c>
+      <c r="D15">
+        <v>5801</v>
+      </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
@@ -3113,8 +3515,11 @@
       <c r="G15">
         <v>1607</v>
       </c>
+      <c r="H15">
+        <v>1575</v>
+      </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3124,6 +3529,9 @@
       <c r="C16">
         <v>10074</v>
       </c>
+      <c r="D16">
+        <v>8221</v>
+      </c>
       <c r="E16" t="s">
         <v>14</v>
       </c>
@@ -3133,8 +3541,11 @@
       <c r="G16">
         <v>3171</v>
       </c>
+      <c r="H16">
+        <v>2990</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3144,6 +3555,9 @@
       <c r="C17">
         <v>10272</v>
       </c>
+      <c r="D17">
+        <v>7756</v>
+      </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
@@ -3153,8 +3567,11 @@
       <c r="G17">
         <v>3440</v>
       </c>
+      <c r="H17">
+        <v>2938</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3164,6 +3581,9 @@
       <c r="C18">
         <v>7184</v>
       </c>
+      <c r="D18">
+        <v>6061</v>
+      </c>
       <c r="E18" t="s">
         <v>16</v>
       </c>
@@ -3173,8 +3593,11 @@
       <c r="G18">
         <v>2191</v>
       </c>
+      <c r="H18">
+        <v>1698</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3184,6 +3607,9 @@
       <c r="C19">
         <v>6766</v>
       </c>
+      <c r="D19">
+        <v>5473</v>
+      </c>
       <c r="E19" t="s">
         <v>17</v>
       </c>
@@ -3192,6 +3618,9 @@
       </c>
       <c r="G19">
         <v>1654</v>
+      </c>
+      <c r="H19">
+        <v>1516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix the small bug
</commit_message>
<xml_diff>
--- a/comparison/comparison.xlsx
+++ b/comparison/comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\EPFL\course\gsoc\scala-native-autotest\comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89B8436-9DA7-480E-BE6D-7CE59170E944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB37A0FD-F602-4902-938A-5ED565440462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2988" yWindow="1488" windowWidth="17280" windowHeight="9420" xr2:uid="{0F7EB116-8E3E-4DAC-9B80-7CB50F2397D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0F7EB116-8E3E-4DAC-9B80-7CB50F2397D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>bounce.BounceBenchmark</t>
   </si>
@@ -89,15 +89,14 @@
     <t>tracer.TracerBenchmark</t>
   </si>
   <si>
-    <t>baseline(ms)</t>
+    <t>Baseline (ms)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>inc comp(ms)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Incremental Compilation (ms)</t>
   </si>
   <si>
-    <t>inc comp v2</t>
+    <t>Incremental Compilation (ms)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -200,7 +199,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>first compilation</a:t>
+              <a:t>First Compilation</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN" altLang="en-US"/>
           </a:p>
@@ -251,7 +250,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>baseline(ms)</c:v>
+                  <c:v>Baseline (ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -335,65 +334,65 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>6238</c:v>
+                  <c:v>6394</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5611</c:v>
+                  <c:v>5595</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5494</c:v>
+                  <c:v>5420</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5555</c:v>
+                  <c:v>5247</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5151</c:v>
+                  <c:v>5125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5867</c:v>
+                  <c:v>5923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5350</c:v>
+                  <c:v>5263</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5388</c:v>
+                  <c:v>5136</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5403</c:v>
+                  <c:v>5329</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5166</c:v>
+                  <c:v>5325</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5297</c:v>
+                  <c:v>5467</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5477</c:v>
+                  <c:v>5188</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5849</c:v>
+                  <c:v>5389</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5690</c:v>
+                  <c:v>5271</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7449</c:v>
+                  <c:v>7331</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7564</c:v>
+                  <c:v>7183</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5581</c:v>
+                  <c:v>5287</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5556</c:v>
+                  <c:v>5420</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F2B3-4A6C-90B5-E9AAF7EB7738}"/>
+              <c16:uniqueId val="{00000000-216C-498A-BEE6-9FEECBCFEE1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -406,7 +405,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>inc comp(ms)</c:v>
+                  <c:v>Incremental Compilation (ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -490,220 +489,65 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>7603</c:v>
+                  <c:v>6542</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7079</c:v>
+                  <c:v>6061</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7007</c:v>
+                  <c:v>6179</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6444</c:v>
+                  <c:v>5851</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6654</c:v>
+                  <c:v>5813</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7936</c:v>
+                  <c:v>6409</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6800</c:v>
+                  <c:v>5897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6554</c:v>
+                  <c:v>5944</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6395</c:v>
+                  <c:v>5901</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6334</c:v>
+                  <c:v>5931</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6629</c:v>
+                  <c:v>5847</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6768</c:v>
+                  <c:v>5824</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6394</c:v>
+                  <c:v>6007</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6610</c:v>
+                  <c:v>5801</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10074</c:v>
+                  <c:v>8221</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10272</c:v>
+                  <c:v>7756</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7184</c:v>
+                  <c:v>6061</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6766</c:v>
+                  <c:v>5473</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F2B3-4A6C-90B5-E9AAF7EB7738}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>inc comp v2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>bounce.BounceBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>brainfuck.BrainfuckBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>cd.CDBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>deltablue.DeltaBlueBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>gcbench.GCBenchBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>histogram.Histogram</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>json.JsonBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>kmeans.KmeansBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>list.ListBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>mandelbrot.MandelbrotBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>nbody.NbodyBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>permute.PermuteBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>queens.QueensBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>richards.RichardsBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>rsc.RscBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>rsc.cli.Main</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>sudoku.SudokuBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>tracer.TracerBenchmark</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>6542</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6061</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6179</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5851</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5813</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6409</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5897</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5944</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5901</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5931</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5847</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5824</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6007</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5801</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8221</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7756</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>6061</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5473</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B3C1-4F88-A495-3DDEEB1AC4A4}"/>
+              <c16:uniqueId val="{00000001-216C-498A-BEE6-9FEECBCFEE1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -716,11 +560,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="823490784"/>
-        <c:axId val="823493280"/>
+        <c:axId val="1168425024"/>
+        <c:axId val="1168400480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="823490784"/>
+        <c:axId val="1168425024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -763,7 +607,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="823493280"/>
+        <c:crossAx val="1168400480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -771,7 +615,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="823493280"/>
+        <c:axId val="1168400480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,7 +666,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="823490784"/>
+        <c:crossAx val="1168425024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -944,7 +788,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>later compilations</a:t>
+              <a:t>Later Compilation</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN" altLang="en-US"/>
           </a:p>
@@ -995,7 +839,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>baseline(ms)</c:v>
+                  <c:v>Baseline (ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1079,65 +923,65 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2309</c:v>
+                  <c:v>2351</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2237</c:v>
+                  <c:v>2149</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2007</c:v>
+                  <c:v>2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1969</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2751</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1944</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1858</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1867</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1881</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1926</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1942</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2513</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1930</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1928</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="14">
+                  <c:v>3948</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3904</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2150</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>1974</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1927</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2042</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2082</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2086</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1908</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4031</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5003</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2196</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FD64-4516-8707-1A2851169988}"/>
+              <c16:uniqueId val="{00000000-44F7-4D1A-903E-EA2455F78616}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1150,7 +994,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>inc comp(ms)</c:v>
+                  <c:v>Incremental Compilation (ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1234,220 +1078,65 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1940</c:v>
+                  <c:v>1952</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1841</c:v>
+                  <c:v>1757</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1686</c:v>
+                  <c:v>1636</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1673</c:v>
+                  <c:v>1626</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1637</c:v>
+                  <c:v>1521</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2144</c:v>
+                  <c:v>1909</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1627</c:v>
+                  <c:v>1610</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1631</c:v>
+                  <c:v>1512</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1598</c:v>
+                  <c:v>1636</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1626</c:v>
+                  <c:v>1523</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1735</c:v>
+                  <c:v>1587</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1619</c:v>
+                  <c:v>1527</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1623</c:v>
+                  <c:v>1482</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1607</c:v>
+                  <c:v>1575</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3171</c:v>
+                  <c:v>2990</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3440</c:v>
+                  <c:v>2938</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2191</c:v>
+                  <c:v>1698</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1654</c:v>
+                  <c:v>1516</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FD64-4516-8707-1A2851169988}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>inc comp v2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$E$2:$E$19</c:f>
-              <c:strCache>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>bounce.BounceBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>brainfuck.BrainfuckBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>cd.CDBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>deltablue.DeltaBlueBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>gcbench.GCBenchBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>histogram.Histogram</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>json.JsonBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>kmeans.KmeansBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>list.ListBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>mandelbrot.MandelbrotBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>nbody.NbodyBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>permute.PermuteBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>queens.QueensBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>richards.RichardsBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>rsc.RscBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>rsc.cli.Main</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>sudoku.SudokuBenchmark</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>tracer.TracerBenchmark</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$2:$H$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>1952</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1757</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1636</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1626</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1521</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1909</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1610</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1512</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1636</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1523</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1587</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1527</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1482</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1575</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2990</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2938</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1698</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1516</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E3B0-4306-BDE1-2532922F712B}"/>
+              <c16:uniqueId val="{00000001-44F7-4D1A-903E-EA2455F78616}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1460,11 +1149,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="991194480"/>
-        <c:axId val="991194896"/>
+        <c:axId val="916203216"/>
+        <c:axId val="916199888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="991194480"/>
+        <c:axId val="916203216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1507,7 +1196,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="991194896"/>
+        <c:crossAx val="916199888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1515,7 +1204,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="991194896"/>
+        <c:axId val="916199888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,7 +1255,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="991194480"/>
+        <c:crossAx val="916203216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2748,22 +2437,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:colOff>1241611</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>170329</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>61257</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>125505</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="图表 1">
+        <xdr:cNvPr id="4" name="图表 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADDDB070-7903-7C3E-79C7-68E88547C17A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C2DFE70-1D13-0AE6-E80D-72E25EA498EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2784,22 +2473,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>1008528</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>125506</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>410880</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>80682</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="图表 2">
+        <xdr:cNvPr id="5" name="图表 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6718E331-99ED-1E14-4363-0A21E4F1C0E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A4164B1-4FD2-CA9F-77EC-8523593C7965}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3117,32 +2806,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F046F08D-F85D-44BC-BED6-982A55F38414}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.88671875" customWidth="1"/>
     <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="27.33203125" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="29.88671875" customWidth="1"/>
     <col min="8" max="8" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
         <v>20</v>
       </c>
       <c r="F1" t="s">
@@ -3151,475 +2837,364 @@
       <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>6238</v>
+        <v>6394</v>
       </c>
       <c r="C2">
-        <v>7603</v>
-      </c>
-      <c r="D2">
         <v>6542</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>2309</v>
+        <v>2351</v>
       </c>
       <c r="G2">
-        <v>1940</v>
-      </c>
-      <c r="H2">
         <v>1952</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5611</v>
+        <v>5595</v>
       </c>
       <c r="C3">
-        <v>7079</v>
-      </c>
-      <c r="D3">
         <v>6061</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>2237</v>
+        <v>2149</v>
       </c>
       <c r="G3">
-        <v>1841</v>
-      </c>
-      <c r="H3">
         <v>1757</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5494</v>
+        <v>5420</v>
       </c>
       <c r="C4">
-        <v>7007</v>
-      </c>
-      <c r="D4">
         <v>6179</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>2007</v>
+        <v>2022</v>
       </c>
       <c r="G4">
-        <v>1686</v>
-      </c>
-      <c r="H4">
         <v>1636</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5555</v>
+        <v>5247</v>
       </c>
       <c r="C5">
-        <v>6444</v>
-      </c>
-      <c r="D5">
         <v>5851</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>1926</v>
+        <v>2042</v>
       </c>
       <c r="G5">
-        <v>1673</v>
-      </c>
-      <c r="H5">
         <v>1626</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5151</v>
+        <v>5125</v>
       </c>
       <c r="C6">
-        <v>6654</v>
-      </c>
-      <c r="D6">
         <v>5813</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>1942</v>
+        <v>1969</v>
       </c>
       <c r="G6">
-        <v>1637</v>
-      </c>
-      <c r="H6">
         <v>1521</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5867</v>
+        <v>5923</v>
       </c>
       <c r="C7">
-        <v>7936</v>
-      </c>
-      <c r="D7">
         <v>6409</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>2513</v>
+        <v>2751</v>
       </c>
       <c r="G7">
-        <v>2144</v>
-      </c>
-      <c r="H7">
         <v>1909</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5350</v>
+        <v>5263</v>
       </c>
       <c r="C8">
-        <v>6800</v>
-      </c>
-      <c r="D8">
         <v>5897</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>1930</v>
+        <v>1944</v>
       </c>
       <c r="G8">
-        <v>1627</v>
-      </c>
-      <c r="H8">
         <v>1610</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>5388</v>
+        <v>5136</v>
       </c>
       <c r="C9">
-        <v>6554</v>
-      </c>
-      <c r="D9">
         <v>5944</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
       </c>
       <c r="F9">
-        <v>1928</v>
+        <v>2044</v>
       </c>
       <c r="G9">
-        <v>1631</v>
-      </c>
-      <c r="H9">
         <v>1512</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>5403</v>
+        <v>5329</v>
       </c>
       <c r="C10">
-        <v>6395</v>
-      </c>
-      <c r="D10">
         <v>5901</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
       <c r="F10">
-        <v>1974</v>
+        <v>1858</v>
       </c>
       <c r="G10">
-        <v>1598</v>
-      </c>
-      <c r="H10">
         <v>1636</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5166</v>
+        <v>5325</v>
       </c>
       <c r="C11">
-        <v>6334</v>
-      </c>
-      <c r="D11">
         <v>5931</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>1927</v>
+        <v>1978</v>
       </c>
       <c r="G11">
-        <v>1626</v>
-      </c>
-      <c r="H11">
         <v>1523</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>5297</v>
+        <v>5467</v>
       </c>
       <c r="C12">
-        <v>6629</v>
-      </c>
-      <c r="D12">
         <v>5847</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
       </c>
       <c r="F12">
-        <v>2042</v>
+        <v>2012</v>
       </c>
       <c r="G12">
-        <v>1735</v>
-      </c>
-      <c r="H12">
         <v>1587</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>5477</v>
+        <v>5188</v>
       </c>
       <c r="C13">
-        <v>6768</v>
-      </c>
-      <c r="D13">
         <v>5824</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
       <c r="F13">
-        <v>2082</v>
+        <v>1867</v>
       </c>
       <c r="G13">
-        <v>1619</v>
-      </c>
-      <c r="H13">
         <v>1527</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>5849</v>
+        <v>5389</v>
       </c>
       <c r="C14">
-        <v>6394</v>
-      </c>
-      <c r="D14">
         <v>6007</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
       </c>
       <c r="F14">
-        <v>2086</v>
+        <v>1881</v>
       </c>
       <c r="G14">
-        <v>1623</v>
-      </c>
-      <c r="H14">
         <v>1482</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>5690</v>
+        <v>5271</v>
       </c>
       <c r="C15">
-        <v>6610</v>
-      </c>
-      <c r="D15">
         <v>5801</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
       <c r="F15">
-        <v>1908</v>
+        <v>1926</v>
       </c>
       <c r="G15">
-        <v>1607</v>
-      </c>
-      <c r="H15">
         <v>1575</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>7449</v>
+        <v>7331</v>
       </c>
       <c r="C16">
-        <v>10074</v>
-      </c>
-      <c r="D16">
         <v>8221</v>
       </c>
       <c r="E16" t="s">
         <v>14</v>
       </c>
       <c r="F16">
-        <v>4031</v>
+        <v>3948</v>
       </c>
       <c r="G16">
-        <v>3171</v>
-      </c>
-      <c r="H16">
         <v>2990</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>7564</v>
+        <v>7183</v>
       </c>
       <c r="C17">
-        <v>10272</v>
-      </c>
-      <c r="D17">
         <v>7756</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17">
-        <v>5003</v>
+        <v>3904</v>
       </c>
       <c r="G17">
-        <v>3440</v>
-      </c>
-      <c r="H17">
         <v>2938</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>5581</v>
+        <v>5287</v>
       </c>
       <c r="C18">
-        <v>7184</v>
-      </c>
-      <c r="D18">
         <v>6061</v>
       </c>
       <c r="E18" t="s">
         <v>16</v>
       </c>
       <c r="F18">
-        <v>2196</v>
+        <v>2150</v>
       </c>
       <c r="G18">
-        <v>2191</v>
-      </c>
-      <c r="H18">
         <v>1698</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>5556</v>
+        <v>5420</v>
       </c>
       <c r="C19">
-        <v>6766</v>
-      </c>
-      <c r="D19">
         <v>5473</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
       </c>
       <c r="F19">
-        <v>1992</v>
+        <v>1974</v>
       </c>
       <c r="G19">
-        <v>1654</v>
-      </c>
-      <c r="H19">
         <v>1516</v>
       </c>
     </row>

</xml_diff>